<commit_message>
Changed file structure so it is more orgainzed
</commit_message>
<xml_diff>
--- a/data/ListSort_AgeAdjxlsx.xlsx
+++ b/data/ListSort_AgeAdjxlsx.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\InternQX\Movie-HCP_Brain_Graph-master\Movie-HCP_Brain_Graph-master- test\Movie-HCP_Brain_Graph-master-test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\InternQX\Movie-HCP_Brain_Graph-master\Movie-HCP_Brain_Graph-master- test\Movie-HCP_Brain_Graph-master-test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{313B3078-73C5-42EB-A3AB-EF81F13FCAA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0811A0B-BA74-4992-A8A2-7F20ADAB23F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{982F0155-47DF-455B-917F-AC80AAC66809}"/>
   </bookViews>
@@ -393,16 +393,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{686E158A-B776-41D7-83F7-E1A24719741C}">
   <dimension ref="A1:B185"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -410,7 +410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>100610</v>
       </c>
@@ -418,7 +418,7 @@
         <v>108.26</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>102311</v>
       </c>
@@ -426,7 +426,7 @@
         <v>113.85</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>102816</v>
       </c>
@@ -434,7 +434,7 @@
         <v>112.66</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>104416</v>
       </c>
@@ -442,7 +442,7 @@
         <v>102.63</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>105923</v>
       </c>
@@ -450,7 +450,7 @@
         <v>112.66</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>108323</v>
       </c>
@@ -458,7 +458,7 @@
         <v>98.44</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>109123</v>
       </c>
@@ -466,7 +466,7 @@
         <v>131.78</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>111312</v>
       </c>
@@ -474,7 +474,7 @@
         <v>102.63</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>111514</v>
       </c>
@@ -482,7 +482,7 @@
         <v>102.63</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>114823</v>
       </c>
@@ -490,7 +490,7 @@
         <v>122.75</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>115017</v>
       </c>
@@ -498,7 +498,7 @@
         <v>97.6</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>115825</v>
       </c>
@@ -506,7 +506,7 @@
         <v>94.33</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>116726</v>
       </c>
@@ -514,7 +514,7 @@
         <v>118.14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>118225</v>
       </c>
@@ -522,7 +522,7 @@
         <v>123.73</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>125525</v>
       </c>
@@ -530,7 +530,7 @@
         <v>80.14</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>126426</v>
       </c>
@@ -538,7 +538,7 @@
         <v>102.63</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>126931</v>
       </c>
@@ -546,7 +546,7 @@
         <v>97.6</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>128935</v>
       </c>
@@ -554,7 +554,7 @@
         <v>107.32</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>130114</v>
       </c>
@@ -562,7 +562,7 @@
         <v>98.44</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>130518</v>
       </c>
@@ -570,7 +570,7 @@
         <v>88.33</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>131217</v>
       </c>
@@ -578,7 +578,7 @@
         <v>84.01</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>131722</v>
       </c>
@@ -586,7 +586,7 @@
         <v>122.75</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>132118</v>
       </c>
@@ -594,7 +594,7 @@
         <v>89.14</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>134627</v>
       </c>
@@ -602,7 +602,7 @@
         <v>94.33</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>134829</v>
       </c>
@@ -610,7 +610,7 @@
         <v>97.6</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>135124</v>
       </c>
@@ -618,7 +618,7 @@
         <v>102.63</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>137128</v>
       </c>
@@ -626,7 +626,7 @@
         <v>127.41</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>140117</v>
       </c>
@@ -634,7 +634,7 @@
         <v>98.44</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>144226</v>
       </c>
@@ -642,7 +642,7 @@
         <v>75.819999999999993</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>145834</v>
       </c>
@@ -650,7 +650,7 @@
         <v>118.14</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>146129</v>
       </c>
@@ -658,7 +658,7 @@
         <v>108.26</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>146432</v>
       </c>
@@ -666,7 +666,7 @@
         <v>93.3</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>146735</v>
       </c>
@@ -674,7 +674,7 @@
         <v>93.3</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>146937</v>
       </c>
@@ -682,7 +682,7 @@
         <v>102.63</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>148133</v>
       </c>
@@ -690,7 +690,7 @@
         <v>103.57</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>150423</v>
       </c>
@@ -698,7 +698,7 @@
         <v>102.63</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>155938</v>
       </c>
@@ -706,7 +706,7 @@
         <v>98.44</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>156334</v>
       </c>
@@ -714,7 +714,7 @@
         <v>89.14</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>157336</v>
       </c>
@@ -722,7 +722,7 @@
         <v>69.099999999999994</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>158035</v>
       </c>
@@ -730,7 +730,7 @@
         <v>69.099999999999994</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>158136</v>
       </c>
@@ -738,7 +738,7 @@
         <v>84.01</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>159239</v>
       </c>
@@ -746,7 +746,7 @@
         <v>117.24</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>162935</v>
       </c>
@@ -754,7 +754,7 @@
         <v>94.33</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>164131</v>
       </c>
@@ -762,7 +762,7 @@
         <v>118.14</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>164636</v>
       </c>
@@ -770,7 +770,7 @@
         <v>132.49</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>165436</v>
       </c>
@@ -778,7 +778,7 @@
         <v>103.57</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>167036</v>
       </c>
@@ -786,7 +786,7 @@
         <v>93.3</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>167440</v>
       </c>
@@ -794,7 +794,7 @@
         <v>84.01</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>169040</v>
       </c>
@@ -802,7 +802,7 @@
         <v>98.44</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>169343</v>
       </c>
@@ -810,7 +810,7 @@
         <v>75.819999999999993</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>169444</v>
       </c>
@@ -818,7 +818,7 @@
         <v>97.6</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>169747</v>
       </c>
@@ -826,7 +826,7 @@
         <v>102.63</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>171633</v>
       </c>
@@ -834,7 +834,7 @@
         <v>85.26</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>172130</v>
       </c>
@@ -842,7 +842,7 @@
         <v>103.57</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>173334</v>
       </c>
@@ -850,7 +850,7 @@
         <v>128.24</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>175237</v>
       </c>
@@ -858,7 +858,7 @@
         <v>127.41</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>176542</v>
       </c>
@@ -866,7 +866,7 @@
         <v>103.57</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>177140</v>
       </c>
@@ -874,7 +874,7 @@
         <v>112.66</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>177645</v>
       </c>
@@ -882,7 +882,7 @@
         <v>98.44</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>177746</v>
       </c>
@@ -890,7 +890,7 @@
         <v>107.32</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>178142</v>
       </c>
@@ -898,7 +898,7 @@
         <v>113.85</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>178243</v>
       </c>
@@ -906,7 +906,7 @@
         <v>98.44</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>178647</v>
       </c>
@@ -914,7 +914,7 @@
         <v>93.3</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>180533</v>
       </c>
@@ -922,7 +922,7 @@
         <v>102.63</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>181232</v>
       </c>
@@ -930,7 +930,7 @@
         <v>103.57</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>181636</v>
       </c>
@@ -938,7 +938,7 @@
         <v>88.33</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>182436</v>
       </c>
@@ -946,7 +946,7 @@
         <v>84.01</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>182739</v>
       </c>
@@ -954,7 +954,7 @@
         <v>97.6</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>185442</v>
       </c>
@@ -962,7 +962,7 @@
         <v>98.44</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>186949</v>
       </c>
@@ -970,7 +970,7 @@
         <v>103.57</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>187345</v>
       </c>
@@ -978,7 +978,7 @@
         <v>122.75</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>191033</v>
       </c>
@@ -986,7 +986,7 @@
         <v>94.33</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>191336</v>
       </c>
@@ -994,7 +994,7 @@
         <v>122.75</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>191841</v>
       </c>
@@ -1002,7 +1002,7 @@
         <v>103.57</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>192439</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>75.819999999999993</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>192641</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>107.32</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>193845</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>103.57</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>195041</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>93.3</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>196144</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>107.32</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>197348</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>97.6</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>198653</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>108.26</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>199655</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>102.63</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>200210</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>118.14</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>200311</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>107.32</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>200614</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>84.01</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>201515</v>
       </c>
@@ -1098,7 +1098,7 @@
         <v>103.57</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>203418</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>94.33</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>204521</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>97.6</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>205220</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>107.32</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>209228</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>98.44</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>212419</v>
       </c>
@@ -1138,7 +1138,7 @@
         <v>89.14</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>214019</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>112.66</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>214524</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>123.73</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>221319</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>72.900000000000006</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>233326</v>
       </c>
@@ -1170,7 +1170,7 @@
         <v>112.66</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>239136</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>84.01</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>246133</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>98.44</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>249947</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>88.33</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>251833</v>
       </c>
@@ -1202,7 +1202,7 @@
         <v>102.63</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>257845</v>
       </c>
@@ -1210,7 +1210,7 @@
         <v>108.26</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>263436</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>93.3</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>283543</v>
       </c>
@@ -1226,7 +1226,7 @@
         <v>89.14</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>318637</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>103.57</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>320826</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>93.3</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>330324</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>108.26</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>346137</v>
       </c>
@@ -1258,7 +1258,7 @@
         <v>112.66</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>352738</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>112.66</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>360030</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>107.32</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>365343</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>102.63</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>380036</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>113.85</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>381038</v>
       </c>
@@ -1298,7 +1298,7 @@
         <v>93.3</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>385046</v>
       </c>
@@ -1306,7 +1306,7 @@
         <v>80.7</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>389357</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>108.26</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>393247</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>107.32</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>395756</v>
       </c>
@@ -1330,7 +1330,7 @@
         <v>84.01</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>397760</v>
       </c>
@@ -1338,7 +1338,7 @@
         <v>97.6</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>401422</v>
       </c>
@@ -1346,7 +1346,7 @@
         <v>127.41</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>406836</v>
       </c>
@@ -1354,7 +1354,7 @@
         <v>112.66</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>412528</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>93.3</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>429040</v>
       </c>
@@ -1370,7 +1370,7 @@
         <v>62.34</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>436845</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>85.26</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>463040</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>102.63</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>467351</v>
       </c>
@@ -1394,7 +1394,7 @@
         <v>112.66</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>473952</v>
       </c>
@@ -1402,7 +1402,7 @@
         <v>112.66</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>525541</v>
       </c>
@@ -1410,7 +1410,7 @@
         <v>102.63</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>536647</v>
       </c>
@@ -1418,7 +1418,7 @@
         <v>88.33</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>541943</v>
       </c>
@@ -1426,7 +1426,7 @@
         <v>103.57</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>547046</v>
       </c>
@@ -1434,7 +1434,7 @@
         <v>113.85</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>550439</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>80.7</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>552241</v>
       </c>
@@ -1450,7 +1450,7 @@
         <v>85.26</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>562345</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>84.01</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>572045</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>97.6</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>573249</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>117.24</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>581450</v>
       </c>
@@ -1482,7 +1482,7 @@
         <v>108.26</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>585256</v>
       </c>
@@ -1490,7 +1490,7 @@
         <v>75.819999999999993</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>601127</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>123.73</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>617748</v>
       </c>
@@ -1506,7 +1506,7 @@
         <v>102.63</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>627549</v>
       </c>
@@ -1514,7 +1514,7 @@
         <v>88.33</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>638049</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>107.32</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>644246</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>112.66</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>654552</v>
       </c>
@@ -1538,7 +1538,7 @@
         <v>107.32</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>671855</v>
       </c>
@@ -1546,7 +1546,7 @@
         <v>113.85</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>680957</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>107.32</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>690152</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>112.66</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>706040</v>
       </c>
@@ -1570,7 +1570,7 @@
         <v>98.44</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>724446</v>
       </c>
@@ -1578,7 +1578,7 @@
         <v>113.85</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>725751</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>113.85</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>732243</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>117.24</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>745555</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>88.33</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>751550</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>93.3</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>757764</v>
       </c>
@@ -1618,7 +1618,7 @@
         <v>112.66</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>765864</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>113.85</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>770352</v>
       </c>
@@ -1634,7 +1634,7 @@
         <v>97.6</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>771354</v>
       </c>
@@ -1642,7 +1642,7 @@
         <v>123.73</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>782561</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>102.63</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>783462</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>113.85</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>789373</v>
       </c>
@@ -1666,7 +1666,7 @@
         <v>118.14</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>814649</v>
       </c>
@@ -1674,7 +1674,7 @@
         <v>98.44</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>818859</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>93.3</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>825048</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>117.24</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>826353</v>
       </c>
@@ -1698,7 +1698,7 @@
         <v>102.63</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>833249</v>
       </c>
@@ -1706,7 +1706,7 @@
         <v>98.44</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>859671</v>
       </c>
@@ -1714,7 +1714,7 @@
         <v>127.41</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>861456</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>93.3</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>871762</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>123.73</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>872764</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>89.14</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>878776</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>113.85</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>878877</v>
       </c>
@@ -1754,7 +1754,7 @@
         <v>66.489999999999995</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>898176</v>
       </c>
@@ -1762,7 +1762,7 @@
         <v>102.63</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>899885</v>
       </c>
@@ -1770,7 +1770,7 @@
         <v>108.26</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>901139</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>118.14</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>901442</v>
       </c>
@@ -1786,7 +1786,7 @@
         <v>102.63</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>905147</v>
       </c>
@@ -1794,7 +1794,7 @@
         <v>102.63</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>910241</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>112.66</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>926862</v>
       </c>
@@ -1810,7 +1810,7 @@
         <v>118.14</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>927359</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>118.14</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>942658</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>122.75</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>943862</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>94.33</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>951457</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>80.14</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>958976</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>98.44</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>966975</v>
       </c>
@@ -1858,7 +1858,7 @@
         <v>98.44</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>971160</v>
       </c>
@@ -1866,7 +1866,7 @@
         <v>98.44</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>973770</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>80.7</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>995174</v>
       </c>

</xml_diff>